<commit_message>
fix the error encode value in pid
</commit_message>
<xml_diff>
--- a/pidDebug.xlsx
+++ b/pidDebug.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3574" uniqueCount="1486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3616" uniqueCount="1526">
   <si>
     <t>success MPU6050 init</t>
   </si>
@@ -4481,6 +4482,130 @@
   </si>
   <si>
     <t xml:space="preserve">gYroY = 36.201221 </t>
+  </si>
+  <si>
+    <t>yA[0]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yA[1]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yA[2]</t>
+  </si>
+  <si>
+    <t>yA[3]</t>
+  </si>
+  <si>
+    <t>yA[4]</t>
+  </si>
+  <si>
+    <t>yA[5]</t>
+  </si>
+  <si>
+    <t>yA[6]</t>
+  </si>
+  <si>
+    <t>yA[7]</t>
+  </si>
+  <si>
+    <t>yA[8]</t>
+  </si>
+  <si>
+    <t>yA[9]</t>
+  </si>
+  <si>
+    <t>yA[10]</t>
+  </si>
+  <si>
+    <t>yA[11]</t>
+  </si>
+  <si>
+    <t>yA[12]</t>
+  </si>
+  <si>
+    <t>yA[13]</t>
+  </si>
+  <si>
+    <t>yA[14]</t>
+  </si>
+  <si>
+    <t>yA[15]</t>
+  </si>
+  <si>
+    <t>yA[16]</t>
+  </si>
+  <si>
+    <t>yA[17]</t>
+  </si>
+  <si>
+    <t>yA[18]</t>
+  </si>
+  <si>
+    <t>yA[19]</t>
+  </si>
+  <si>
+    <t>pA[0]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pA[1]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pA[2]</t>
+  </si>
+  <si>
+    <t>pA[3]</t>
+  </si>
+  <si>
+    <t>pA[4]</t>
+  </si>
+  <si>
+    <t>pA[5]</t>
+  </si>
+  <si>
+    <t>pA[6]</t>
+  </si>
+  <si>
+    <t>pA[7]</t>
+  </si>
+  <si>
+    <t>pA[8]</t>
+  </si>
+  <si>
+    <t>pA[9]</t>
+  </si>
+  <si>
+    <t>pA[10]</t>
+  </si>
+  <si>
+    <t>pA[11]</t>
+  </si>
+  <si>
+    <t>pA[12]</t>
+  </si>
+  <si>
+    <t>pA[13]</t>
+  </si>
+  <si>
+    <t>pA[14]</t>
+  </si>
+  <si>
+    <t>pA[15]</t>
+  </si>
+  <si>
+    <t>pA[16]</t>
+  </si>
+  <si>
+    <t>pA[17]</t>
+  </si>
+  <si>
+    <t>pA[18]</t>
+  </si>
+  <si>
+    <t>pA[19]</t>
   </si>
 </sst>
 </file>
@@ -4529,10 +4654,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -11842,8 +11970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+    <sheetView tabSelected="1" topLeftCell="B70" workbookViewId="0">
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -16404,4 +16532,2018 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.59765625" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="4.59765625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1487</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1488</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1489</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>1490</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>1491</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>1492</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>1493</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>1494</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>1495</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>1496</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>1497</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>1498</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>1499</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>1500</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>1501</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>1502</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>1503</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>1504</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>976</v>
+      </c>
+      <c r="B4" s="3">
+        <v>974</v>
+      </c>
+      <c r="C4" s="3">
+        <v>987</v>
+      </c>
+      <c r="D4" s="3">
+        <v>991</v>
+      </c>
+      <c r="E4" s="3">
+        <v>996</v>
+      </c>
+      <c r="F4" s="3">
+        <v>999</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1000</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1002</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1006</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1007</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1013</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1021</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1025</v>
+      </c>
+      <c r="N4" s="3">
+        <v>1034</v>
+      </c>
+      <c r="O4" s="3">
+        <v>1036</v>
+      </c>
+      <c r="P4" s="3">
+        <v>1038</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>1038</v>
+      </c>
+      <c r="R4" s="3">
+        <v>1044</v>
+      </c>
+      <c r="S4" s="3">
+        <v>1051</v>
+      </c>
+      <c r="T4" s="3">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>1080</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1080</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1076</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1077</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1076</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1077</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1077</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1077</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1077</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1077</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1079</v>
+      </c>
+      <c r="L5" s="3">
+        <v>1077</v>
+      </c>
+      <c r="M5" s="3">
+        <v>1076</v>
+      </c>
+      <c r="N5" s="3">
+        <v>1079</v>
+      </c>
+      <c r="O5" s="3">
+        <v>1077</v>
+      </c>
+      <c r="P5" s="3">
+        <v>1078</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>1080</v>
+      </c>
+      <c r="R5" s="3">
+        <v>1077</v>
+      </c>
+      <c r="S5" s="3">
+        <v>1077</v>
+      </c>
+      <c r="T5" s="3">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>1075</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1076</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1076</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1077</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1077</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1076</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1075</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1076</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1076</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1078</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1075</v>
+      </c>
+      <c r="L6" s="3">
+        <v>1078</v>
+      </c>
+      <c r="M6" s="3">
+        <v>1075</v>
+      </c>
+      <c r="N6" s="3">
+        <v>1075</v>
+      </c>
+      <c r="O6" s="3">
+        <v>1075</v>
+      </c>
+      <c r="P6" s="3">
+        <v>1075</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>1075</v>
+      </c>
+      <c r="R6" s="3">
+        <v>1075</v>
+      </c>
+      <c r="S6" s="3">
+        <v>1074</v>
+      </c>
+      <c r="T6" s="3">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>1070</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1070</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1070</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1071</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1074</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1070</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1071</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1074</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1072</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1072</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1071</v>
+      </c>
+      <c r="L7" s="3">
+        <v>1072</v>
+      </c>
+      <c r="M7" s="3">
+        <v>1071</v>
+      </c>
+      <c r="N7" s="3">
+        <v>1071</v>
+      </c>
+      <c r="O7" s="3">
+        <v>1073</v>
+      </c>
+      <c r="P7" s="3">
+        <v>1070</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>1071</v>
+      </c>
+      <c r="R7" s="3">
+        <v>1073</v>
+      </c>
+      <c r="S7" s="3">
+        <v>1070</v>
+      </c>
+      <c r="T7" s="3">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>1072</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1072</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1072</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1071</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1074</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1073</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1071</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1073</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1070</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1070</v>
+      </c>
+      <c r="K8" s="3">
+        <v>1073</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1075</v>
+      </c>
+      <c r="M8" s="3">
+        <v>1074</v>
+      </c>
+      <c r="N8" s="3">
+        <v>1075</v>
+      </c>
+      <c r="O8" s="3">
+        <v>1073</v>
+      </c>
+      <c r="P8" s="3">
+        <v>1074</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>1073</v>
+      </c>
+      <c r="R8" s="3">
+        <v>1074</v>
+      </c>
+      <c r="S8" s="3">
+        <v>1071</v>
+      </c>
+      <c r="T8" s="3">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>1074</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1075</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1073</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1075</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1075</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1074</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1075</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1073</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1074</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1072</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1074</v>
+      </c>
+      <c r="L9" s="3">
+        <v>1074</v>
+      </c>
+      <c r="M9" s="3">
+        <v>1072</v>
+      </c>
+      <c r="N9" s="3">
+        <v>1074</v>
+      </c>
+      <c r="O9" s="3">
+        <v>1075</v>
+      </c>
+      <c r="P9" s="3">
+        <v>1073</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>1072</v>
+      </c>
+      <c r="R9" s="3">
+        <v>1075</v>
+      </c>
+      <c r="S9" s="3">
+        <v>1074</v>
+      </c>
+      <c r="T9" s="3">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>1075</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1075</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1077</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1078</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1076</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1076</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1073</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1076</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1078</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1075</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1075</v>
+      </c>
+      <c r="L10" s="3">
+        <v>1078</v>
+      </c>
+      <c r="M10" s="3">
+        <v>1076</v>
+      </c>
+      <c r="N10" s="3">
+        <v>1078</v>
+      </c>
+      <c r="O10" s="3">
+        <v>1076</v>
+      </c>
+      <c r="P10" s="3">
+        <v>1077</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>1074</v>
+      </c>
+      <c r="R10" s="3">
+        <v>1075</v>
+      </c>
+      <c r="S10" s="3">
+        <v>1077</v>
+      </c>
+      <c r="T10" s="3">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>1074</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1072</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1075</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1074</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1075</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1075</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1075</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1074</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1074</v>
+      </c>
+      <c r="J11" s="3">
+        <v>1076</v>
+      </c>
+      <c r="K11" s="3">
+        <v>1074</v>
+      </c>
+      <c r="L11" s="3">
+        <v>1074</v>
+      </c>
+      <c r="M11" s="3">
+        <v>1078</v>
+      </c>
+      <c r="N11" s="3">
+        <v>1073</v>
+      </c>
+      <c r="O11" s="3">
+        <v>1073</v>
+      </c>
+      <c r="P11" s="3">
+        <v>1075</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>1076</v>
+      </c>
+      <c r="R11" s="3">
+        <v>1075</v>
+      </c>
+      <c r="S11" s="3">
+        <v>1075</v>
+      </c>
+      <c r="T11" s="3">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>1076</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1076</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1076</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1073</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1075</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1076</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1075</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1074</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1077</v>
+      </c>
+      <c r="K12" s="3">
+        <v>1074</v>
+      </c>
+      <c r="L12" s="3">
+        <v>1076</v>
+      </c>
+      <c r="M12" s="3">
+        <v>1076</v>
+      </c>
+      <c r="N12" s="3">
+        <v>1073</v>
+      </c>
+      <c r="O12" s="3">
+        <v>1077</v>
+      </c>
+      <c r="P12" s="3">
+        <v>1075</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>1075</v>
+      </c>
+      <c r="R12" s="3">
+        <v>1072</v>
+      </c>
+      <c r="S12" s="3">
+        <v>1073</v>
+      </c>
+      <c r="T12" s="3">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>1075</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1075</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1075</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1073</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1076</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1076</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1075</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1076</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1075</v>
+      </c>
+      <c r="J13" s="3">
+        <v>1076</v>
+      </c>
+      <c r="K13" s="3">
+        <v>1075</v>
+      </c>
+      <c r="L13" s="3">
+        <v>1074</v>
+      </c>
+      <c r="M13" s="3">
+        <v>1073</v>
+      </c>
+      <c r="N13" s="3">
+        <v>1077</v>
+      </c>
+      <c r="O13" s="3">
+        <v>1076</v>
+      </c>
+      <c r="P13" s="3">
+        <v>1075</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>1074</v>
+      </c>
+      <c r="R13" s="3">
+        <v>1078</v>
+      </c>
+      <c r="S13" s="3">
+        <v>1075</v>
+      </c>
+      <c r="T13" s="3">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>1071</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1071</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1072</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1073</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1073</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1073</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1073</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1075</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1073</v>
+      </c>
+      <c r="J14" s="3">
+        <v>1074</v>
+      </c>
+      <c r="K14" s="3">
+        <v>1072</v>
+      </c>
+      <c r="L14" s="3">
+        <v>1073</v>
+      </c>
+      <c r="M14" s="3">
+        <v>1075</v>
+      </c>
+      <c r="N14" s="3">
+        <v>1074</v>
+      </c>
+      <c r="O14" s="3">
+        <v>1073</v>
+      </c>
+      <c r="P14" s="3">
+        <v>1073</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>1075</v>
+      </c>
+      <c r="R14" s="3">
+        <v>1075</v>
+      </c>
+      <c r="S14" s="3">
+        <v>1074</v>
+      </c>
+      <c r="T14" s="3">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>1072</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1072</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1072</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1075</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1073</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1071</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1073</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1075</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1074</v>
+      </c>
+      <c r="J15" s="3">
+        <v>1074</v>
+      </c>
+      <c r="K15" s="3">
+        <v>1074</v>
+      </c>
+      <c r="L15" s="3">
+        <v>1073</v>
+      </c>
+      <c r="M15" s="3">
+        <v>1072</v>
+      </c>
+      <c r="N15" s="3">
+        <v>1073</v>
+      </c>
+      <c r="O15" s="3">
+        <v>1074</v>
+      </c>
+      <c r="P15" s="3">
+        <v>1075</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>1073</v>
+      </c>
+      <c r="R15" s="3">
+        <v>1074</v>
+      </c>
+      <c r="S15" s="3">
+        <v>1072</v>
+      </c>
+      <c r="T15" s="3">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>1075</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1075</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1074</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1075</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1073</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1074</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1071</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1073</v>
+      </c>
+      <c r="I16" s="3">
+        <v>1074</v>
+      </c>
+      <c r="J16" s="3">
+        <v>1074</v>
+      </c>
+      <c r="K16" s="3">
+        <v>1072</v>
+      </c>
+      <c r="L16" s="3">
+        <v>1075</v>
+      </c>
+      <c r="M16" s="3">
+        <v>1074</v>
+      </c>
+      <c r="N16" s="3">
+        <v>1076</v>
+      </c>
+      <c r="O16" s="3">
+        <v>1074</v>
+      </c>
+      <c r="P16" s="3">
+        <v>1075</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>1074</v>
+      </c>
+      <c r="R16" s="3">
+        <v>1076</v>
+      </c>
+      <c r="S16" s="3">
+        <v>1073</v>
+      </c>
+      <c r="T16" s="3">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>1075</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1074</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1073</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1074</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1071</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1075</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1074</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1073</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1072</v>
+      </c>
+      <c r="J17" s="3">
+        <v>1073</v>
+      </c>
+      <c r="K17" s="3">
+        <v>1072</v>
+      </c>
+      <c r="L17" s="3">
+        <v>1072</v>
+      </c>
+      <c r="M17" s="3">
+        <v>1073</v>
+      </c>
+      <c r="N17" s="3">
+        <v>1076</v>
+      </c>
+      <c r="O17" s="3">
+        <v>1074</v>
+      </c>
+      <c r="P17" s="3">
+        <v>1073</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>1074</v>
+      </c>
+      <c r="R17" s="3">
+        <v>1075</v>
+      </c>
+      <c r="S17" s="3">
+        <v>1075</v>
+      </c>
+      <c r="T17" s="3">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>1072</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1072</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1072</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1074</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1072</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1071</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1074</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1071</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1072</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1070</v>
+      </c>
+      <c r="K18" s="3">
+        <v>1071</v>
+      </c>
+      <c r="L18" s="3">
+        <v>1073</v>
+      </c>
+      <c r="M18" s="3">
+        <v>1074</v>
+      </c>
+      <c r="N18" s="3">
+        <v>1071</v>
+      </c>
+      <c r="O18" s="3">
+        <v>1071</v>
+      </c>
+      <c r="P18" s="3">
+        <v>1076</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>1076</v>
+      </c>
+      <c r="R18" s="3">
+        <v>1074</v>
+      </c>
+      <c r="S18" s="3">
+        <v>1073</v>
+      </c>
+      <c r="T18" s="3">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>1506</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>1507</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>1509</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>1510</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>1511</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>1512</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>1513</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>1514</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>1515</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>1516</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>1517</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>1518</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>1519</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>1520</v>
+      </c>
+      <c r="P22" s="3" t="s">
+        <v>1521</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>1522</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>1523</v>
+      </c>
+      <c r="S22" s="3" t="s">
+        <v>1524</v>
+      </c>
+      <c r="T22" s="3" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>1486</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1486</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1489</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1495</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1499</v>
+      </c>
+      <c r="F23" s="3">
+        <v>1502</v>
+      </c>
+      <c r="G23" s="3">
+        <v>1499</v>
+      </c>
+      <c r="H23" s="3">
+        <v>1498</v>
+      </c>
+      <c r="I23" s="3">
+        <v>1497</v>
+      </c>
+      <c r="J23" s="3">
+        <v>1497</v>
+      </c>
+      <c r="K23" s="3">
+        <v>1498</v>
+      </c>
+      <c r="L23" s="3">
+        <v>1497</v>
+      </c>
+      <c r="M23" s="3">
+        <v>1496</v>
+      </c>
+      <c r="N23" s="3">
+        <v>1497</v>
+      </c>
+      <c r="O23" s="3">
+        <v>1497</v>
+      </c>
+      <c r="P23" s="3">
+        <v>1496</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>1498</v>
+      </c>
+      <c r="R23" s="3">
+        <v>1496</v>
+      </c>
+      <c r="S23" s="3">
+        <v>1494</v>
+      </c>
+      <c r="T23" s="3">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>554</v>
+      </c>
+      <c r="B24" s="3">
+        <v>554</v>
+      </c>
+      <c r="C24" s="3">
+        <v>555</v>
+      </c>
+      <c r="D24" s="3">
+        <v>556</v>
+      </c>
+      <c r="E24" s="3">
+        <v>556</v>
+      </c>
+      <c r="F24" s="3">
+        <v>555</v>
+      </c>
+      <c r="G24" s="3">
+        <v>554</v>
+      </c>
+      <c r="H24" s="3">
+        <v>555</v>
+      </c>
+      <c r="I24" s="3">
+        <v>554</v>
+      </c>
+      <c r="J24" s="3">
+        <v>555</v>
+      </c>
+      <c r="K24" s="3">
+        <v>556</v>
+      </c>
+      <c r="L24" s="3">
+        <v>556</v>
+      </c>
+      <c r="M24" s="3">
+        <v>556</v>
+      </c>
+      <c r="N24" s="3">
+        <v>557</v>
+      </c>
+      <c r="O24" s="3">
+        <v>558</v>
+      </c>
+      <c r="P24" s="3">
+        <v>557</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>557</v>
+      </c>
+      <c r="R24" s="3">
+        <v>558</v>
+      </c>
+      <c r="S24" s="3">
+        <v>557</v>
+      </c>
+      <c r="T24" s="3">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>557</v>
+      </c>
+      <c r="B25" s="3">
+        <v>557</v>
+      </c>
+      <c r="C25" s="3">
+        <v>557</v>
+      </c>
+      <c r="D25" s="3">
+        <v>556</v>
+      </c>
+      <c r="E25" s="3">
+        <v>557</v>
+      </c>
+      <c r="F25" s="3">
+        <v>556</v>
+      </c>
+      <c r="G25" s="3">
+        <v>556</v>
+      </c>
+      <c r="H25" s="3">
+        <v>556</v>
+      </c>
+      <c r="I25" s="3">
+        <v>555</v>
+      </c>
+      <c r="J25" s="3">
+        <v>556</v>
+      </c>
+      <c r="K25" s="3">
+        <v>557</v>
+      </c>
+      <c r="L25" s="3">
+        <v>557</v>
+      </c>
+      <c r="M25" s="3">
+        <v>556</v>
+      </c>
+      <c r="N25" s="3">
+        <v>557</v>
+      </c>
+      <c r="O25" s="3">
+        <v>556</v>
+      </c>
+      <c r="P25" s="3">
+        <v>557</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>557</v>
+      </c>
+      <c r="R25" s="3">
+        <v>557</v>
+      </c>
+      <c r="S25" s="3">
+        <v>557</v>
+      </c>
+      <c r="T25" s="3">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>558</v>
+      </c>
+      <c r="B26" s="3">
+        <v>555</v>
+      </c>
+      <c r="C26" s="3">
+        <v>555</v>
+      </c>
+      <c r="D26" s="3">
+        <v>555</v>
+      </c>
+      <c r="E26" s="3">
+        <v>555</v>
+      </c>
+      <c r="F26" s="3">
+        <v>556</v>
+      </c>
+      <c r="G26" s="3">
+        <v>559</v>
+      </c>
+      <c r="H26" s="3">
+        <v>558</v>
+      </c>
+      <c r="I26" s="3">
+        <v>557</v>
+      </c>
+      <c r="J26" s="3">
+        <v>558</v>
+      </c>
+      <c r="K26" s="3">
+        <v>559</v>
+      </c>
+      <c r="L26" s="3">
+        <v>557</v>
+      </c>
+      <c r="M26" s="3">
+        <v>556</v>
+      </c>
+      <c r="N26" s="3">
+        <v>558</v>
+      </c>
+      <c r="O26" s="3">
+        <v>558</v>
+      </c>
+      <c r="P26" s="3">
+        <v>558</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>558</v>
+      </c>
+      <c r="R26" s="3">
+        <v>560</v>
+      </c>
+      <c r="S26" s="3">
+        <v>559</v>
+      </c>
+      <c r="T26" s="3">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>562</v>
+      </c>
+      <c r="B27" s="3">
+        <v>562</v>
+      </c>
+      <c r="C27" s="3">
+        <v>563</v>
+      </c>
+      <c r="D27" s="3">
+        <v>561</v>
+      </c>
+      <c r="E27" s="3">
+        <v>562</v>
+      </c>
+      <c r="F27" s="3">
+        <v>562</v>
+      </c>
+      <c r="G27" s="3">
+        <v>559</v>
+      </c>
+      <c r="H27" s="3">
+        <v>561</v>
+      </c>
+      <c r="I27" s="3">
+        <v>560</v>
+      </c>
+      <c r="J27" s="3">
+        <v>562</v>
+      </c>
+      <c r="K27" s="3">
+        <v>560</v>
+      </c>
+      <c r="L27" s="3">
+        <v>561</v>
+      </c>
+      <c r="M27" s="3">
+        <v>561</v>
+      </c>
+      <c r="N27" s="3">
+        <v>560</v>
+      </c>
+      <c r="O27" s="3">
+        <v>561</v>
+      </c>
+      <c r="P27" s="3">
+        <v>560</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>560</v>
+      </c>
+      <c r="R27" s="3">
+        <v>558</v>
+      </c>
+      <c r="S27" s="3">
+        <v>561</v>
+      </c>
+      <c r="T27" s="3">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>557</v>
+      </c>
+      <c r="B28" s="3">
+        <v>556</v>
+      </c>
+      <c r="C28" s="3">
+        <v>555</v>
+      </c>
+      <c r="D28" s="3">
+        <v>555</v>
+      </c>
+      <c r="E28" s="3">
+        <v>555</v>
+      </c>
+      <c r="F28" s="3">
+        <v>557</v>
+      </c>
+      <c r="G28" s="3">
+        <v>554</v>
+      </c>
+      <c r="H28" s="3">
+        <v>556</v>
+      </c>
+      <c r="I28" s="3">
+        <v>555</v>
+      </c>
+      <c r="J28" s="3">
+        <v>557</v>
+      </c>
+      <c r="K28" s="3">
+        <v>557</v>
+      </c>
+      <c r="L28" s="3">
+        <v>555</v>
+      </c>
+      <c r="M28" s="3">
+        <v>556</v>
+      </c>
+      <c r="N28" s="3">
+        <v>556</v>
+      </c>
+      <c r="O28" s="3">
+        <v>555</v>
+      </c>
+      <c r="P28" s="3">
+        <v>558</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>556</v>
+      </c>
+      <c r="R28" s="3">
+        <v>556</v>
+      </c>
+      <c r="S28" s="3">
+        <v>557</v>
+      </c>
+      <c r="T28" s="3">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>558</v>
+      </c>
+      <c r="B29" s="3">
+        <v>558</v>
+      </c>
+      <c r="C29" s="3">
+        <v>558</v>
+      </c>
+      <c r="D29" s="3">
+        <v>560</v>
+      </c>
+      <c r="E29" s="3">
+        <v>559</v>
+      </c>
+      <c r="F29" s="3">
+        <v>558</v>
+      </c>
+      <c r="G29" s="3">
+        <v>557</v>
+      </c>
+      <c r="H29" s="3">
+        <v>557</v>
+      </c>
+      <c r="I29" s="3">
+        <v>558</v>
+      </c>
+      <c r="J29" s="3">
+        <v>560</v>
+      </c>
+      <c r="K29" s="3">
+        <v>558</v>
+      </c>
+      <c r="L29" s="3">
+        <v>559</v>
+      </c>
+      <c r="M29" s="3">
+        <v>560</v>
+      </c>
+      <c r="N29" s="3">
+        <v>559</v>
+      </c>
+      <c r="O29" s="3">
+        <v>559</v>
+      </c>
+      <c r="P29" s="3">
+        <v>559</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>559</v>
+      </c>
+      <c r="R29" s="3">
+        <v>559</v>
+      </c>
+      <c r="S29" s="3">
+        <v>560</v>
+      </c>
+      <c r="T29" s="3">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>555</v>
+      </c>
+      <c r="B30" s="3">
+        <v>554</v>
+      </c>
+      <c r="C30" s="3">
+        <v>554</v>
+      </c>
+      <c r="D30" s="3">
+        <v>553</v>
+      </c>
+      <c r="E30" s="3">
+        <v>553</v>
+      </c>
+      <c r="F30" s="3">
+        <v>553</v>
+      </c>
+      <c r="G30" s="3">
+        <v>554</v>
+      </c>
+      <c r="H30" s="3">
+        <v>554</v>
+      </c>
+      <c r="I30" s="3">
+        <v>553</v>
+      </c>
+      <c r="J30" s="3">
+        <v>555</v>
+      </c>
+      <c r="K30" s="3">
+        <v>555</v>
+      </c>
+      <c r="L30" s="3">
+        <v>556</v>
+      </c>
+      <c r="M30" s="3">
+        <v>556</v>
+      </c>
+      <c r="N30" s="3">
+        <v>556</v>
+      </c>
+      <c r="O30" s="3">
+        <v>556</v>
+      </c>
+      <c r="P30" s="3">
+        <v>555</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>554</v>
+      </c>
+      <c r="R30" s="3">
+        <v>552</v>
+      </c>
+      <c r="S30" s="3">
+        <v>554</v>
+      </c>
+      <c r="T30" s="3">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>561</v>
+      </c>
+      <c r="B31" s="3">
+        <v>561</v>
+      </c>
+      <c r="C31" s="3">
+        <v>561</v>
+      </c>
+      <c r="D31" s="3">
+        <v>561</v>
+      </c>
+      <c r="E31" s="3">
+        <v>561</v>
+      </c>
+      <c r="F31" s="3">
+        <v>562</v>
+      </c>
+      <c r="G31" s="3">
+        <v>561</v>
+      </c>
+      <c r="H31" s="3">
+        <v>559</v>
+      </c>
+      <c r="I31" s="3">
+        <v>560</v>
+      </c>
+      <c r="J31" s="3">
+        <v>562</v>
+      </c>
+      <c r="K31" s="3">
+        <v>559</v>
+      </c>
+      <c r="L31" s="3">
+        <v>559</v>
+      </c>
+      <c r="M31" s="3">
+        <v>561</v>
+      </c>
+      <c r="N31" s="3">
+        <v>559</v>
+      </c>
+      <c r="O31" s="3">
+        <v>560</v>
+      </c>
+      <c r="P31" s="3">
+        <v>560</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>559</v>
+      </c>
+      <c r="R31" s="3">
+        <v>559</v>
+      </c>
+      <c r="S31" s="3">
+        <v>559</v>
+      </c>
+      <c r="T31" s="3">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>551</v>
+      </c>
+      <c r="B32" s="3">
+        <v>551</v>
+      </c>
+      <c r="C32" s="3">
+        <v>550</v>
+      </c>
+      <c r="D32" s="3">
+        <v>550</v>
+      </c>
+      <c r="E32" s="3">
+        <v>550</v>
+      </c>
+      <c r="F32" s="3">
+        <v>551</v>
+      </c>
+      <c r="G32" s="3">
+        <v>553</v>
+      </c>
+      <c r="H32" s="3">
+        <v>552</v>
+      </c>
+      <c r="I32" s="3">
+        <v>552</v>
+      </c>
+      <c r="J32" s="3">
+        <v>553</v>
+      </c>
+      <c r="K32" s="3">
+        <v>553</v>
+      </c>
+      <c r="L32" s="3">
+        <v>554</v>
+      </c>
+      <c r="M32" s="3">
+        <v>552</v>
+      </c>
+      <c r="N32" s="3">
+        <v>554</v>
+      </c>
+      <c r="O32" s="3">
+        <v>555</v>
+      </c>
+      <c r="P32" s="3">
+        <v>554</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>554</v>
+      </c>
+      <c r="R32" s="3">
+        <v>554</v>
+      </c>
+      <c r="S32" s="3">
+        <v>554</v>
+      </c>
+      <c r="T32" s="3">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>561</v>
+      </c>
+      <c r="B33" s="3">
+        <v>561</v>
+      </c>
+      <c r="C33" s="3">
+        <v>560</v>
+      </c>
+      <c r="D33" s="3">
+        <v>561</v>
+      </c>
+      <c r="E33" s="3">
+        <v>559</v>
+      </c>
+      <c r="F33" s="3">
+        <v>561</v>
+      </c>
+      <c r="G33" s="3">
+        <v>561</v>
+      </c>
+      <c r="H33" s="3">
+        <v>560</v>
+      </c>
+      <c r="I33" s="3">
+        <v>559</v>
+      </c>
+      <c r="J33" s="3">
+        <v>561</v>
+      </c>
+      <c r="K33" s="3">
+        <v>560</v>
+      </c>
+      <c r="L33" s="3">
+        <v>561</v>
+      </c>
+      <c r="M33" s="3">
+        <v>559</v>
+      </c>
+      <c r="N33" s="3">
+        <v>561</v>
+      </c>
+      <c r="O33" s="3">
+        <v>558</v>
+      </c>
+      <c r="P33" s="3">
+        <v>560</v>
+      </c>
+      <c r="Q33" s="3">
+        <v>559</v>
+      </c>
+      <c r="R33" s="3">
+        <v>559</v>
+      </c>
+      <c r="S33" s="3">
+        <v>560</v>
+      </c>
+      <c r="T33" s="3">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>556</v>
+      </c>
+      <c r="B34" s="3">
+        <v>556</v>
+      </c>
+      <c r="C34" s="3">
+        <v>556</v>
+      </c>
+      <c r="D34" s="3">
+        <v>556</v>
+      </c>
+      <c r="E34" s="3">
+        <v>556</v>
+      </c>
+      <c r="F34" s="3">
+        <v>556</v>
+      </c>
+      <c r="G34" s="3">
+        <v>556</v>
+      </c>
+      <c r="H34" s="3">
+        <v>556</v>
+      </c>
+      <c r="I34" s="3">
+        <v>555</v>
+      </c>
+      <c r="J34" s="3">
+        <v>557</v>
+      </c>
+      <c r="K34" s="3">
+        <v>557</v>
+      </c>
+      <c r="L34" s="3">
+        <v>556</v>
+      </c>
+      <c r="M34" s="3">
+        <v>556</v>
+      </c>
+      <c r="N34" s="3">
+        <v>555</v>
+      </c>
+      <c r="O34" s="3">
+        <v>556</v>
+      </c>
+      <c r="P34" s="3">
+        <v>557</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>556</v>
+      </c>
+      <c r="R34" s="3">
+        <v>558</v>
+      </c>
+      <c r="S34" s="3">
+        <v>556</v>
+      </c>
+      <c r="T34" s="3">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>573</v>
+      </c>
+      <c r="B35" s="3">
+        <v>573</v>
+      </c>
+      <c r="C35" s="3">
+        <v>573</v>
+      </c>
+      <c r="D35" s="3">
+        <v>574</v>
+      </c>
+      <c r="E35" s="3">
+        <v>573</v>
+      </c>
+      <c r="F35" s="3">
+        <v>572</v>
+      </c>
+      <c r="G35" s="3">
+        <v>569</v>
+      </c>
+      <c r="H35" s="3">
+        <v>568</v>
+      </c>
+      <c r="I35" s="3">
+        <v>566</v>
+      </c>
+      <c r="J35" s="3">
+        <v>566</v>
+      </c>
+      <c r="K35" s="3">
+        <v>566</v>
+      </c>
+      <c r="L35" s="3">
+        <v>565</v>
+      </c>
+      <c r="M35" s="3">
+        <v>563</v>
+      </c>
+      <c r="N35" s="3">
+        <v>565</v>
+      </c>
+      <c r="O35" s="3">
+        <v>564</v>
+      </c>
+      <c r="P35" s="3">
+        <v>565</v>
+      </c>
+      <c r="Q35" s="3">
+        <v>564</v>
+      </c>
+      <c r="R35" s="3">
+        <v>565</v>
+      </c>
+      <c r="S35" s="3">
+        <v>565</v>
+      </c>
+      <c r="T35" s="3">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>565</v>
+      </c>
+      <c r="B36" s="3">
+        <v>565</v>
+      </c>
+      <c r="C36" s="3">
+        <v>566</v>
+      </c>
+      <c r="D36" s="3">
+        <v>564</v>
+      </c>
+      <c r="E36" s="3">
+        <v>566</v>
+      </c>
+      <c r="F36" s="3">
+        <v>565</v>
+      </c>
+      <c r="G36" s="3">
+        <v>564</v>
+      </c>
+      <c r="H36" s="3">
+        <v>563</v>
+      </c>
+      <c r="I36" s="3">
+        <v>563</v>
+      </c>
+      <c r="J36" s="3">
+        <v>562</v>
+      </c>
+      <c r="K36" s="3">
+        <v>562</v>
+      </c>
+      <c r="L36" s="3">
+        <v>562</v>
+      </c>
+      <c r="M36" s="3">
+        <v>561</v>
+      </c>
+      <c r="N36" s="3">
+        <v>561</v>
+      </c>
+      <c r="O36" s="3">
+        <v>560</v>
+      </c>
+      <c r="P36" s="3">
+        <v>561</v>
+      </c>
+      <c r="Q36" s="3">
+        <v>563</v>
+      </c>
+      <c r="R36" s="3">
+        <v>562</v>
+      </c>
+      <c r="S36" s="3">
+        <v>563</v>
+      </c>
+      <c r="T36" s="3">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
+        <v>564</v>
+      </c>
+      <c r="B37" s="3">
+        <v>564</v>
+      </c>
+      <c r="C37" s="3">
+        <v>564</v>
+      </c>
+      <c r="D37" s="3">
+        <v>565</v>
+      </c>
+      <c r="E37" s="3">
+        <v>566</v>
+      </c>
+      <c r="F37" s="3">
+        <v>564</v>
+      </c>
+      <c r="G37" s="3">
+        <v>564</v>
+      </c>
+      <c r="H37" s="3">
+        <v>564</v>
+      </c>
+      <c r="I37" s="3">
+        <v>565</v>
+      </c>
+      <c r="J37" s="3">
+        <v>564</v>
+      </c>
+      <c r="K37" s="3">
+        <v>563</v>
+      </c>
+      <c r="L37" s="3">
+        <v>561</v>
+      </c>
+      <c r="M37" s="3">
+        <v>564</v>
+      </c>
+      <c r="N37" s="3">
+        <v>561</v>
+      </c>
+      <c r="O37" s="3">
+        <v>561</v>
+      </c>
+      <c r="P37" s="3">
+        <v>562</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>563</v>
+      </c>
+      <c r="R37" s="3">
+        <v>561</v>
+      </c>
+      <c r="S37" s="3">
+        <v>561</v>
+      </c>
+      <c r="T37" s="3">
+        <v>561</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>